<commit_message>
All Expenses Refined the expense category
</commit_message>
<xml_diff>
--- a/1_udemy_course/my_custom_data/All_Expense_Category_Lookup.xlsx
+++ b/1_udemy_course/my_custom_data/All_Expense_Category_Lookup.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Naveen_Data\Power_Bi\power_bi\1_udemy_course\my_custom_data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="23895" windowHeight="9975"/>
   </bookViews>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="107">
   <si>
     <t>Sub-Category</t>
   </si>
@@ -331,13 +336,22 @@
   </si>
   <si>
     <t>Reimbursement</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GoldMakingChrg </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -381,6 +395,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -427,7 +449,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -459,9 +481,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -493,6 +516,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -668,14 +692,15 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:D74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="C81" sqref="C81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
@@ -683,7 +708,7 @@
     <col min="4" max="4" width="32.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -697,7 +722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -711,7 +736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -725,7 +750,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -739,7 +764,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -753,7 +778,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>11</v>
       </c>
@@ -767,7 +792,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -781,7 +806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>15</v>
       </c>
@@ -795,12 +820,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:4">
+    <row r="9" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>5</v>
+        <v>104</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
@@ -809,7 +834,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
@@ -823,7 +848,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -837,7 +862,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>24</v>
       </c>
@@ -845,13 +870,13 @@
         <v>5</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>10</v>
+        <v>106</v>
       </c>
       <c r="D12" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>25</v>
       </c>
@@ -865,7 +890,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>27</v>
       </c>
@@ -879,7 +904,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>29</v>
       </c>
@@ -893,7 +918,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>30</v>
       </c>
@@ -907,7 +932,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>32</v>
       </c>
@@ -921,7 +946,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>34</v>
       </c>
@@ -935,7 +960,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:4">
+    <row r="19" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>35</v>
       </c>
@@ -949,7 +974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
         <v>37</v>
       </c>
@@ -963,7 +988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
@@ -977,7 +1002,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:4">
+    <row r="22" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>40</v>
       </c>
@@ -991,7 +1016,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>41</v>
       </c>
@@ -1005,7 +1030,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4">
+    <row r="24" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>42</v>
       </c>
@@ -1019,7 +1044,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>44</v>
       </c>
@@ -1033,7 +1058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>46</v>
       </c>
@@ -1047,7 +1072,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>47</v>
       </c>
@@ -1061,7 +1086,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
         <v>49</v>
       </c>
@@ -1075,7 +1100,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>50</v>
       </c>
@@ -1089,7 +1114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:4">
+    <row r="30" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>51</v>
       </c>
@@ -1103,7 +1128,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>53</v>
       </c>
@@ -1117,7 +1142,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:4">
+    <row r="32" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>54</v>
       </c>
@@ -1131,7 +1156,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:4">
+    <row r="33" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>55</v>
       </c>
@@ -1145,7 +1170,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="1:4">
+    <row r="34" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>57</v>
       </c>
@@ -1159,7 +1184,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:4">
+    <row r="35" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>59</v>
       </c>
@@ -1173,7 +1198,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4">
+    <row r="36" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
         <v>60</v>
       </c>
@@ -1187,7 +1212,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:4">
+    <row r="37" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>62</v>
       </c>
@@ -1201,7 +1226,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4">
+    <row r="38" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
         <v>64</v>
       </c>
@@ -1215,7 +1240,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:4">
+    <row r="39" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>65</v>
       </c>
@@ -1229,7 +1254,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:4">
+    <row r="40" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
         <v>66</v>
       </c>
@@ -1243,7 +1268,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:4">
+    <row r="41" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
         <v>67</v>
       </c>
@@ -1257,7 +1282,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:4">
+    <row r="42" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
         <v>68</v>
       </c>
@@ -1271,7 +1296,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:4">
+    <row r="43" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
         <v>69</v>
       </c>
@@ -1285,7 +1310,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:4">
+    <row r="44" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
         <v>70</v>
       </c>
@@ -1299,7 +1324,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:4">
+    <row r="45" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
         <v>71</v>
       </c>
@@ -1313,7 +1338,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
         <v>72</v>
       </c>
@@ -1327,12 +1352,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="47" spans="1:4">
+    <row r="47" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
         <v>73</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>74</v>
@@ -1341,7 +1366,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
+    <row r="48" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
         <v>75</v>
       </c>
@@ -1355,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:4">
+    <row r="49" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>76</v>
       </c>
@@ -1369,7 +1394,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="50" spans="1:4">
+    <row r="50" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
         <v>77</v>
       </c>
@@ -1383,7 +1408,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:4">
+    <row r="51" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
         <v>79</v>
       </c>
@@ -1397,7 +1422,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:4">
+    <row r="52" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
         <v>80</v>
       </c>
@@ -1411,7 +1436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
+    <row r="53" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>81</v>
       </c>
@@ -1425,7 +1450,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="54" spans="1:4">
+    <row r="54" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
         <v>82</v>
       </c>
@@ -1439,7 +1464,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:4">
+    <row r="55" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
         <v>84</v>
       </c>
@@ -1453,7 +1478,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="56" spans="1:4">
+    <row r="56" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
         <v>85</v>
       </c>
@@ -1467,12 +1492,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:4">
+    <row r="57" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>74</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>74</v>
@@ -1481,7 +1506,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
+    <row r="58" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
         <v>86</v>
       </c>
@@ -1495,7 +1520,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="59" spans="1:4">
+    <row r="59" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
         <v>87</v>
       </c>
@@ -1509,7 +1534,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="60" spans="1:4">
+    <row r="60" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
         <v>88</v>
       </c>
@@ -1523,7 +1548,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:4">
+    <row r="61" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
         <v>89</v>
       </c>
@@ -1537,7 +1562,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="62" spans="1:4">
+    <row r="62" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
         <v>90</v>
       </c>
@@ -1551,7 +1576,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
+    <row r="63" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
         <v>92</v>
       </c>
@@ -1565,7 +1590,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="64" spans="1:4">
+    <row r="64" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
         <v>93</v>
       </c>
@@ -1579,12 +1604,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
+    <row r="65" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
         <v>94</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>5</v>
+        <v>105</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>74</v>
@@ -1593,7 +1618,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
+    <row r="66" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
         <v>95</v>
       </c>
@@ -1607,7 +1632,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
+    <row r="67" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
         <v>96</v>
       </c>
@@ -1621,7 +1646,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="68" spans="1:4">
+    <row r="68" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
         <v>97</v>
       </c>
@@ -1635,7 +1660,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:4">
+    <row r="69" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
         <v>98</v>
       </c>
@@ -1649,7 +1674,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="70" spans="1:4">
+    <row r="70" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>99</v>
       </c>
@@ -1663,7 +1688,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="71" spans="1:4">
+    <row r="71" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
         <v>12</v>
       </c>
@@ -1677,7 +1702,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="72" spans="1:4">
+    <row r="72" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
         <v>100</v>
       </c>
@@ -1691,7 +1716,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:4">
+    <row r="73" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
         <v>101</v>
       </c>
@@ -1705,7 +1730,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:4">
+    <row r="74" spans="1:4" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
         <v>102</v>
       </c>
@@ -1720,30 +1745,36 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:D74"/>
+  <autoFilter ref="A1:D74">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="San Cosmetic"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>